<commit_message>
added target and strictness
</commit_message>
<xml_diff>
--- a/data/Neuro_Assays.xlsx
+++ b/data/Neuro_Assays.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/borajin/Documents/BoraJin2018~/Research/DoseResponse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/borajin/Documents/BoraJin2018~/Research/DoseResponse/BMC/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCF7EC7C-10C8-0443-B02D-AC64F62F0DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B51EC0-9BE2-4D40-8E81-5E37F5356EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14980" xr2:uid="{CB2D7CD9-D82C-534F-8435-2FA6BEEB07A2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="345">
   <si>
     <t>assay_name</t>
   </si>
@@ -823,6 +823,255 @@
   </si>
   <si>
     <t>NVS_ENZ_hPDE4D3_Activator</t>
+  </si>
+  <si>
+    <t>intended_target_official_symbol</t>
+  </si>
+  <si>
+    <t>ESR1</t>
+  </si>
+  <si>
+    <t>NR3C1</t>
+  </si>
+  <si>
+    <t>MTF1</t>
+  </si>
+  <si>
+    <t>PAX6</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>PLAUR</t>
+  </si>
+  <si>
+    <t>KDR</t>
+  </si>
+  <si>
+    <t>SERPINE1</t>
+  </si>
+  <si>
+    <t>PLAU</t>
+  </si>
+  <si>
+    <t>IL6</t>
+  </si>
+  <si>
+    <t>CYP19A1</t>
+  </si>
+  <si>
+    <t>ACHE</t>
+  </si>
+  <si>
+    <t>CASP2</t>
+  </si>
+  <si>
+    <t>CSNK2A1</t>
+  </si>
+  <si>
+    <t>MAPK3</t>
+  </si>
+  <si>
+    <t>MARK1</t>
+  </si>
+  <si>
+    <t>MET</t>
+  </si>
+  <si>
+    <t>PDE10A</t>
+  </si>
+  <si>
+    <t>PDE4A</t>
+  </si>
+  <si>
+    <t>PTEN</t>
+  </si>
+  <si>
+    <t>PTPN11</t>
+  </si>
+  <si>
+    <t>Adcy5</t>
+  </si>
+  <si>
+    <t>Comt</t>
+  </si>
+  <si>
+    <t>DYRK1A</t>
+  </si>
+  <si>
+    <t>Maoa</t>
+  </si>
+  <si>
+    <t>Maob</t>
+  </si>
+  <si>
+    <t>DRD1</t>
+  </si>
+  <si>
+    <t>HRH1</t>
+  </si>
+  <si>
+    <t>HTR2A</t>
+  </si>
+  <si>
+    <t>HTR5A</t>
+  </si>
+  <si>
+    <t>HTR7</t>
+  </si>
+  <si>
+    <t>ADRA2A</t>
+  </si>
+  <si>
+    <t>ADRA2C</t>
+  </si>
+  <si>
+    <t>ADRB2</t>
+  </si>
+  <si>
+    <t>DRD2</t>
+  </si>
+  <si>
+    <t>DRD4</t>
+  </si>
+  <si>
+    <t>EDNRB</t>
+  </si>
+  <si>
+    <t>NTSR1</t>
+  </si>
+  <si>
+    <t>AVPR1A</t>
+  </si>
+  <si>
+    <t>HTR2C</t>
+  </si>
+  <si>
+    <t>Htr1a</t>
+  </si>
+  <si>
+    <t>Adra1a</t>
+  </si>
+  <si>
+    <t>Adra1b</t>
+  </si>
+  <si>
+    <t>Adra2a</t>
+  </si>
+  <si>
+    <t>Gabbr1</t>
+  </si>
+  <si>
+    <t>Adra2b</t>
+  </si>
+  <si>
+    <t>Grm1</t>
+  </si>
+  <si>
+    <t>Grm5</t>
+  </si>
+  <si>
+    <t>Tacr1</t>
+  </si>
+  <si>
+    <t>Ntsr1</t>
+  </si>
+  <si>
+    <t>Oxtr</t>
+  </si>
+  <si>
+    <t>Avpr1a</t>
+  </si>
+  <si>
+    <t>Scn1a</t>
+  </si>
+  <si>
+    <t>GABRA1</t>
+  </si>
+  <si>
+    <t>GABRA5</t>
+  </si>
+  <si>
+    <t>HTR3A</t>
+  </si>
+  <si>
+    <t>Gria1</t>
+  </si>
+  <si>
+    <t>Gabra1</t>
+  </si>
+  <si>
+    <t>Grin1</t>
+  </si>
+  <si>
+    <t>Chrna7</t>
+  </si>
+  <si>
+    <t>PGR</t>
+  </si>
+  <si>
+    <t>Esr1</t>
+  </si>
+  <si>
+    <t>Ar</t>
+  </si>
+  <si>
+    <t>FKBP1A</t>
+  </si>
+  <si>
+    <t>SLC6A3</t>
+  </si>
+  <si>
+    <t>SLC6A2</t>
+  </si>
+  <si>
+    <t>SLC6A4</t>
+  </si>
+  <si>
+    <t>Slc6a2</t>
+  </si>
+  <si>
+    <t>Slc6a4</t>
+  </si>
+  <si>
+    <t>NR2F1</t>
+  </si>
+  <si>
+    <t>RORA</t>
+  </si>
+  <si>
+    <t>ADRA1A</t>
+  </si>
+  <si>
+    <t>DRD5</t>
+  </si>
+  <si>
+    <t>GNAQ</t>
+  </si>
+  <si>
+    <t>GNAS</t>
+  </si>
+  <si>
+    <t>GLI3</t>
+  </si>
+  <si>
+    <t>PDE1B</t>
+  </si>
+  <si>
+    <t>PDE4B</t>
+  </si>
+  <si>
+    <t>PDE4D</t>
+  </si>
+  <si>
+    <t>matches to stricter neuro?</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -866,9 +1115,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1183,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E9F4ED4-4352-094E-99B8-44FEF8B75593}">
-  <dimension ref="A1:F177"/>
+  <dimension ref="A1:H177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1197,9 +1452,11 @@
     <col min="4" max="4" width="42.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1218,8 +1475,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1238,8 +1501,14 @@
       <c r="F2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>263</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1258,8 +1527,14 @@
       <c r="F3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>263</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1278,8 +1553,14 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>264</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1298,8 +1579,14 @@
       <c r="F5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>264</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1318,8 +1605,14 @@
       <c r="F6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>265</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1338,8 +1631,14 @@
       <c r="F7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>265</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1358,8 +1657,14 @@
       <c r="F8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>266</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1378,8 +1683,14 @@
       <c r="F9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>266</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1398,8 +1709,14 @@
       <c r="F10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>267</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1418,8 +1735,14 @@
       <c r="F11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>263</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1438,8 +1761,14 @@
       <c r="F12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>264</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1458,8 +1787,14 @@
       <c r="F13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>264</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1478,8 +1813,14 @@
       <c r="F14" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>268</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1498,8 +1839,14 @@
       <c r="F15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>268</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1518,8 +1865,14 @@
       <c r="F16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>268</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1538,8 +1891,14 @@
       <c r="F17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>268</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1558,8 +1917,14 @@
       <c r="F18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>269</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1578,8 +1943,14 @@
       <c r="F19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>269</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>46</v>
       </c>
@@ -1598,8 +1969,14 @@
       <c r="F20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>270</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1618,8 +1995,14 @@
       <c r="F21" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>270</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1638,8 +2021,14 @@
       <c r="F22" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>271</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1658,8 +2047,14 @@
       <c r="F23" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>271</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1678,8 +2073,14 @@
       <c r="F24" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>268</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1698,8 +2099,14 @@
       <c r="F25" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>268</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -1718,8 +2125,14 @@
       <c r="F26" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>272</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>57</v>
       </c>
@@ -1738,8 +2151,14 @@
       <c r="F27" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>272</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -1758,8 +2177,14 @@
       <c r="F28" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" t="s">
+        <v>268</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1778,8 +2203,14 @@
       <c r="F29" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>268</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -1798,8 +2229,14 @@
       <c r="F30" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" t="s">
+        <v>270</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -1818,8 +2255,14 @@
       <c r="F31" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" t="s">
+        <v>270</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -1838,8 +2281,14 @@
       <c r="F32" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" t="s">
+        <v>271</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1858,8 +2307,14 @@
       <c r="F33" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>271</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -1878,8 +2333,14 @@
       <c r="F34" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
+        <v>273</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>73</v>
       </c>
@@ -1898,8 +2359,14 @@
       <c r="F35" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>273</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -1918,8 +2385,14 @@
       <c r="F36" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
+        <v>274</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>76</v>
       </c>
@@ -1938,8 +2411,14 @@
       <c r="F37" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" t="s">
+        <v>274</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -1958,8 +2437,14 @@
       <c r="F38" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" t="s">
+        <v>275</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -1978,8 +2463,14 @@
       <c r="F39" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>275</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>80</v>
       </c>
@@ -1998,8 +2489,14 @@
       <c r="F40" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" t="s">
+        <v>276</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -2018,8 +2515,14 @@
       <c r="F41" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>276</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -2038,8 +2541,14 @@
       <c r="F42" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>277</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -2058,8 +2567,14 @@
       <c r="F43" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
+        <v>277</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>84</v>
       </c>
@@ -2078,8 +2593,14 @@
       <c r="F44" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" t="s">
+        <v>278</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -2098,8 +2619,14 @@
       <c r="F45" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45" t="s">
+        <v>278</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -2118,8 +2645,14 @@
       <c r="F46" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46" t="s">
+        <v>279</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -2138,8 +2671,14 @@
       <c r="F47" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47" t="s">
+        <v>279</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -2158,8 +2697,14 @@
       <c r="F48" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" t="s">
+        <v>280</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -2178,8 +2723,14 @@
       <c r="F49" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" t="s">
+        <v>280</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>90</v>
       </c>
@@ -2198,8 +2749,14 @@
       <c r="F50" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50" t="s">
+        <v>281</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>90</v>
       </c>
@@ -2218,8 +2775,14 @@
       <c r="F51" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51" t="s">
+        <v>281</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>92</v>
       </c>
@@ -2238,8 +2801,14 @@
       <c r="F52" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52" t="s">
+        <v>282</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>92</v>
       </c>
@@ -2258,8 +2827,14 @@
       <c r="F53" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53" t="s">
+        <v>282</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>94</v>
       </c>
@@ -2278,8 +2853,14 @@
       <c r="F54" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54" t="s">
+        <v>283</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>94</v>
       </c>
@@ -2298,8 +2879,14 @@
       <c r="F55" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" t="s">
+        <v>283</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>96</v>
       </c>
@@ -2318,8 +2905,14 @@
       <c r="F56" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56" t="s">
+        <v>269</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>96</v>
       </c>
@@ -2338,8 +2931,14 @@
       <c r="F57" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" t="s">
+        <v>269</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>98</v>
       </c>
@@ -2358,8 +2957,14 @@
       <c r="F58" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58" t="s">
+        <v>284</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>98</v>
       </c>
@@ -2378,8 +2983,14 @@
       <c r="F59" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59" t="s">
+        <v>284</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>102</v>
       </c>
@@ -2398,8 +3009,14 @@
       <c r="F60" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60" t="s">
+        <v>285</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>102</v>
       </c>
@@ -2418,8 +3035,14 @@
       <c r="F61" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61" t="s">
+        <v>285</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>104</v>
       </c>
@@ -2438,8 +3061,14 @@
       <c r="F62" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62" t="s">
+        <v>286</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>104</v>
       </c>
@@ -2458,8 +3087,14 @@
       <c r="F63" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63" t="s">
+        <v>286</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>106</v>
       </c>
@@ -2478,8 +3113,14 @@
       <c r="F64" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64" t="s">
+        <v>287</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>106</v>
       </c>
@@ -2498,8 +3139,14 @@
       <c r="F65" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65" t="s">
+        <v>287</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>108</v>
       </c>
@@ -2518,8 +3165,14 @@
       <c r="F66" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66" t="s">
+        <v>287</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>108</v>
       </c>
@@ -2538,8 +3191,14 @@
       <c r="F67" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67" t="s">
+        <v>287</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>110</v>
       </c>
@@ -2558,8 +3217,14 @@
       <c r="F68" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68" t="s">
+        <v>288</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>110</v>
       </c>
@@ -2578,8 +3243,14 @@
       <c r="F69" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69" t="s">
+        <v>288</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>112</v>
       </c>
@@ -2598,8 +3269,14 @@
       <c r="F70" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70" t="s">
+        <v>288</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>112</v>
       </c>
@@ -2618,8 +3295,14 @@
       <c r="F71" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71" t="s">
+        <v>288</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>114</v>
       </c>
@@ -2638,8 +3321,14 @@
       <c r="F72" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72" t="s">
+        <v>289</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>116</v>
       </c>
@@ -2658,8 +3347,14 @@
       <c r="F73" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73" t="s">
+        <v>290</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>117</v>
       </c>
@@ -2678,8 +3373,14 @@
       <c r="F74" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G74" t="s">
+        <v>291</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>118</v>
       </c>
@@ -2698,8 +3399,14 @@
       <c r="F75" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75" t="s">
+        <v>292</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>119</v>
       </c>
@@ -2718,8 +3425,14 @@
       <c r="F76" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76" t="s">
+        <v>293</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>120</v>
       </c>
@@ -2738,8 +3451,14 @@
       <c r="F77" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77" t="s">
+        <v>294</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>121</v>
       </c>
@@ -2758,8 +3477,14 @@
       <c r="F78" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G78" t="s">
+        <v>295</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>122</v>
       </c>
@@ -2778,8 +3503,14 @@
       <c r="F79" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G79" t="s">
+        <v>296</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>123</v>
       </c>
@@ -2798,8 +3529,14 @@
       <c r="F80" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80" t="s">
+        <v>289</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>124</v>
       </c>
@@ -2818,8 +3555,14 @@
       <c r="F81" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G81" t="s">
+        <v>297</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>125</v>
       </c>
@@ -2838,8 +3581,14 @@
       <c r="F82" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G82" t="s">
+        <v>298</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>126</v>
       </c>
@@ -2858,8 +3607,14 @@
       <c r="F83" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G83" t="s">
+        <v>299</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>127</v>
       </c>
@@ -2878,8 +3633,14 @@
       <c r="F84" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G84" t="s">
+        <v>290</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>128</v>
       </c>
@@ -2898,8 +3659,14 @@
       <c r="F85" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G85" t="s">
+        <v>300</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>129</v>
       </c>
@@ -2918,8 +3685,14 @@
       <c r="F86" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G86" t="s">
+        <v>301</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>130</v>
       </c>
@@ -2938,8 +3711,14 @@
       <c r="F87" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G87" t="s">
+        <v>302</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>132</v>
       </c>
@@ -2958,8 +3737,14 @@
       <c r="F88" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G88" t="s">
+        <v>303</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>133</v>
       </c>
@@ -2978,8 +3763,14 @@
       <c r="F89" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G89" t="s">
+        <v>303</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>134</v>
       </c>
@@ -2998,8 +3789,14 @@
       <c r="F90" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G90" t="s">
+        <v>304</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>135</v>
       </c>
@@ -3018,8 +3815,14 @@
       <c r="F91" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G91" t="s">
+        <v>304</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>136</v>
       </c>
@@ -3038,8 +3841,14 @@
       <c r="F92" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G92" t="s">
+        <v>305</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>137</v>
       </c>
@@ -3058,8 +3867,14 @@
       <c r="F93" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G93" t="s">
+        <v>306</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>138</v>
       </c>
@@ -3078,8 +3893,14 @@
       <c r="F94" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G94" t="s">
+        <v>307</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>139</v>
       </c>
@@ -3098,8 +3919,14 @@
       <c r="F95" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G95" t="s">
+        <v>308</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>140</v>
       </c>
@@ -3118,8 +3945,14 @@
       <c r="F96" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G96" t="s">
+        <v>309</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>141</v>
       </c>
@@ -3138,8 +3971,14 @@
       <c r="F97" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G97" t="s">
+        <v>310</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>142</v>
       </c>
@@ -3158,8 +3997,14 @@
       <c r="F98" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G98" t="s">
+        <v>311</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>144</v>
       </c>
@@ -3178,8 +4023,14 @@
       <c r="F99" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G99" t="s">
+        <v>312</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>145</v>
       </c>
@@ -3198,8 +4049,14 @@
       <c r="F100" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G100" t="s">
+        <v>313</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>147</v>
       </c>
@@ -3218,8 +4075,14 @@
       <c r="F101" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G101" t="s">
+        <v>314</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>148</v>
       </c>
@@ -3238,8 +4101,14 @@
       <c r="F102" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G102" t="s">
+        <v>315</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>149</v>
       </c>
@@ -3258,8 +4127,14 @@
       <c r="F103" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G103" t="s">
+        <v>316</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>150</v>
       </c>
@@ -3278,8 +4153,14 @@
       <c r="F104" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G104" t="s">
+        <v>316</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>151</v>
       </c>
@@ -3298,8 +4179,14 @@
       <c r="F105" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G105" t="s">
+        <v>317</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>152</v>
       </c>
@@ -3318,8 +4205,14 @@
       <c r="F106" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G106" t="s">
+        <v>318</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>153</v>
       </c>
@@ -3338,8 +4231,14 @@
       <c r="F107" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G107" t="s">
+        <v>319</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>154</v>
       </c>
@@ -3358,8 +4257,14 @@
       <c r="F108" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G108" t="s">
+        <v>320</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>155</v>
       </c>
@@ -3378,8 +4283,14 @@
       <c r="F109" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G109" t="s">
+        <v>321</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>156</v>
       </c>
@@ -3398,8 +4309,14 @@
       <c r="F110" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G110" t="s">
+        <v>321</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>157</v>
       </c>
@@ -3418,8 +4335,14 @@
       <c r="F111" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G111" t="s">
+        <v>322</v>
+      </c>
+      <c r="H111" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>158</v>
       </c>
@@ -3438,8 +4361,14 @@
       <c r="F112" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G112" t="s">
+        <v>267</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>159</v>
       </c>
@@ -3458,8 +4387,14 @@
       <c r="F113" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G113" t="s">
+        <v>263</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>160</v>
       </c>
@@ -3478,8 +4413,14 @@
       <c r="F114" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G114" t="s">
+        <v>264</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>161</v>
       </c>
@@ -3498,8 +4439,14 @@
       <c r="F115" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G115" t="s">
+        <v>323</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>162</v>
       </c>
@@ -3518,8 +4465,14 @@
       <c r="F116" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G116" t="s">
+        <v>324</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>164</v>
       </c>
@@ -3538,8 +4491,14 @@
       <c r="F117" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G117" t="s">
+        <v>325</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>166</v>
       </c>
@@ -3558,8 +4517,14 @@
       <c r="F118" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G118" t="s">
+        <v>326</v>
+      </c>
+      <c r="H118" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>167</v>
       </c>
@@ -3578,8 +4543,14 @@
       <c r="F119" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G119" t="s">
+        <v>327</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>168</v>
       </c>
@@ -3598,8 +4569,14 @@
       <c r="F120" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G120" t="s">
+        <v>328</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>169</v>
       </c>
@@ -3618,8 +4595,14 @@
       <c r="F121" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G121" t="s">
+        <v>329</v>
+      </c>
+      <c r="H121" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>170</v>
       </c>
@@ -3638,8 +4621,14 @@
       <c r="F122" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G122" t="s">
+        <v>330</v>
+      </c>
+      <c r="H122" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>171</v>
       </c>
@@ -3658,8 +4647,14 @@
       <c r="F123" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G123" t="s">
+        <v>331</v>
+      </c>
+      <c r="H123" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>172</v>
       </c>
@@ -3678,8 +4673,14 @@
       <c r="F124" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G124" t="s">
+        <v>267</v>
+      </c>
+      <c r="H124" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>175</v>
       </c>
@@ -3698,8 +4699,14 @@
       <c r="F125" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G125" t="s">
+        <v>267</v>
+      </c>
+      <c r="H125" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>177</v>
       </c>
@@ -3718,8 +4725,14 @@
       <c r="F126" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G126" t="s">
+        <v>267</v>
+      </c>
+      <c r="H126" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>178</v>
       </c>
@@ -3738,8 +4751,14 @@
       <c r="F127" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G127" t="s">
+        <v>263</v>
+      </c>
+      <c r="H127" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>179</v>
       </c>
@@ -3758,8 +4777,14 @@
       <c r="F128" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G128" t="s">
+        <v>263</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>180</v>
       </c>
@@ -3778,8 +4803,14 @@
       <c r="F129" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G129" t="s">
+        <v>263</v>
+      </c>
+      <c r="H129" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>183</v>
       </c>
@@ -3798,8 +4829,14 @@
       <c r="F130" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G130" t="s">
+        <v>263</v>
+      </c>
+      <c r="H130" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>185</v>
       </c>
@@ -3818,8 +4855,14 @@
       <c r="F131" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G131" t="s">
+        <v>267</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>187</v>
       </c>
@@ -3838,8 +4881,14 @@
       <c r="F132" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G132" t="s">
+        <v>267</v>
+      </c>
+      <c r="H132" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>189</v>
       </c>
@@ -3858,8 +4907,14 @@
       <c r="F133" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G133" t="s">
+        <v>267</v>
+      </c>
+      <c r="H133" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>190</v>
       </c>
@@ -3878,8 +4933,14 @@
       <c r="F134" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G134" t="s">
+        <v>267</v>
+      </c>
+      <c r="H134" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>191</v>
       </c>
@@ -3898,8 +4959,14 @@
       <c r="F135" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G135" t="s">
+        <v>273</v>
+      </c>
+      <c r="H135" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>192</v>
       </c>
@@ -3918,8 +4985,14 @@
       <c r="F136" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G136" t="s">
+        <v>263</v>
+      </c>
+      <c r="H136" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>194</v>
       </c>
@@ -3938,8 +5011,14 @@
       <c r="F137" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G137" t="s">
+        <v>263</v>
+      </c>
+      <c r="H137" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>196</v>
       </c>
@@ -3958,8 +5037,14 @@
       <c r="F138" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G138" t="s">
+        <v>263</v>
+      </c>
+      <c r="H138" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>197</v>
       </c>
@@ -3978,8 +5063,14 @@
       <c r="F139" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G139" t="s">
+        <v>263</v>
+      </c>
+      <c r="H139" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>198</v>
       </c>
@@ -3998,8 +5089,14 @@
       <c r="F140" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G140" t="s">
+        <v>264</v>
+      </c>
+      <c r="H140" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>200</v>
       </c>
@@ -4018,8 +5115,14 @@
       <c r="F141" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G141" t="s">
+        <v>264</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>202</v>
       </c>
@@ -4038,8 +5141,14 @@
       <c r="F142" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G142" t="s">
+        <v>323</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>202</v>
       </c>
@@ -4058,8 +5167,14 @@
       <c r="F143" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G143" t="s">
+        <v>323</v>
+      </c>
+      <c r="H143" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>202</v>
       </c>
@@ -4078,8 +5193,14 @@
       <c r="F144" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G144" t="s">
+        <v>323</v>
+      </c>
+      <c r="H144" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>202</v>
       </c>
@@ -4098,8 +5219,14 @@
       <c r="F145" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G145" t="s">
+        <v>323</v>
+      </c>
+      <c r="H145" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>211</v>
       </c>
@@ -4118,8 +5245,14 @@
       <c r="F146" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G146" t="s">
+        <v>332</v>
+      </c>
+      <c r="H146" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>211</v>
       </c>
@@ -4138,8 +5271,14 @@
       <c r="F147" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G147" t="s">
+        <v>332</v>
+      </c>
+      <c r="H147" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>211</v>
       </c>
@@ -4158,8 +5297,14 @@
       <c r="F148" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G148" t="s">
+        <v>333</v>
+      </c>
+      <c r="H148" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>211</v>
       </c>
@@ -4178,8 +5323,14 @@
       <c r="F149" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G149" t="s">
+        <v>333</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>211</v>
       </c>
@@ -4198,8 +5349,14 @@
       <c r="F150" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G150" t="s">
+        <v>323</v>
+      </c>
+      <c r="H150" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>220</v>
       </c>
@@ -4218,8 +5375,14 @@
       <c r="F151" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G151" t="s">
+        <v>334</v>
+      </c>
+      <c r="H151" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>220</v>
       </c>
@@ -4238,8 +5401,14 @@
       <c r="F152" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G152" t="s">
+        <v>334</v>
+      </c>
+      <c r="H152" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>220</v>
       </c>
@@ -4258,8 +5427,14 @@
       <c r="F153" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G153" t="s">
+        <v>296</v>
+      </c>
+      <c r="H153" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>220</v>
       </c>
@@ -4278,8 +5453,14 @@
       <c r="F154" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G154" t="s">
+        <v>296</v>
+      </c>
+      <c r="H154" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>220</v>
       </c>
@@ -4298,8 +5479,14 @@
       <c r="F155" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G155" t="s">
+        <v>335</v>
+      </c>
+      <c r="H155" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>220</v>
       </c>
@@ -4318,8 +5505,14 @@
       <c r="F156" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G156" t="s">
+        <v>335</v>
+      </c>
+      <c r="H156" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>220</v>
       </c>
@@ -4338,8 +5531,14 @@
       <c r="F157" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G157" t="s">
+        <v>336</v>
+      </c>
+      <c r="H157" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>220</v>
       </c>
@@ -4358,8 +5557,14 @@
       <c r="F158" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G158" t="s">
+        <v>336</v>
+      </c>
+      <c r="H158" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>220</v>
       </c>
@@ -4378,8 +5583,14 @@
       <c r="F159" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G159" t="s">
+        <v>337</v>
+      </c>
+      <c r="H159" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>220</v>
       </c>
@@ -4398,8 +5609,14 @@
       <c r="F160" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G160" t="s">
+        <v>337</v>
+      </c>
+      <c r="H160" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>220</v>
       </c>
@@ -4418,8 +5635,14 @@
       <c r="F161" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G161" t="s">
+        <v>337</v>
+      </c>
+      <c r="H161" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>220</v>
       </c>
@@ -4438,8 +5661,14 @@
       <c r="F162" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G162" t="s">
+        <v>337</v>
+      </c>
+      <c r="H162" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>220</v>
       </c>
@@ -4458,8 +5687,14 @@
       <c r="F163" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G163" t="s">
+        <v>293</v>
+      </c>
+      <c r="H163" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>220</v>
       </c>
@@ -4478,8 +5713,14 @@
       <c r="F164" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G164" t="s">
+        <v>293</v>
+      </c>
+      <c r="H164" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>242</v>
       </c>
@@ -4498,8 +5739,14 @@
       <c r="F165" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G165" t="s">
+        <v>267</v>
+      </c>
+      <c r="H165" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>244</v>
       </c>
@@ -4518,8 +5765,14 @@
       <c r="F166" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G166" t="s">
+        <v>267</v>
+      </c>
+      <c r="H166" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>247</v>
       </c>
@@ -4538,8 +5791,14 @@
       <c r="F167" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G167" t="s">
+        <v>267</v>
+      </c>
+      <c r="H167" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>249</v>
       </c>
@@ -4558,8 +5817,14 @@
       <c r="F168" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G168" t="s">
+        <v>267</v>
+      </c>
+      <c r="H168" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>251</v>
       </c>
@@ -4578,8 +5843,14 @@
       <c r="F169" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G169" t="s">
+        <v>263</v>
+      </c>
+      <c r="H169" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>253</v>
       </c>
@@ -4598,8 +5869,14 @@
       <c r="F170" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G170" t="s">
+        <v>338</v>
+      </c>
+      <c r="H170" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>255</v>
       </c>
@@ -4618,8 +5895,14 @@
       <c r="F171" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G171" t="s">
+        <v>338</v>
+      </c>
+      <c r="H171" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>256</v>
       </c>
@@ -4638,8 +5921,14 @@
       <c r="F172" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G172" t="s">
+        <v>339</v>
+      </c>
+      <c r="H172" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>256</v>
       </c>
@@ -4658,8 +5947,14 @@
       <c r="F173" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G173" t="s">
+        <v>339</v>
+      </c>
+      <c r="H173" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>258</v>
       </c>
@@ -4678,8 +5973,14 @@
       <c r="F174" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G174" t="s">
+        <v>340</v>
+      </c>
+      <c r="H174" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>258</v>
       </c>
@@ -4698,8 +5999,14 @@
       <c r="F175" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G175" t="s">
+        <v>340</v>
+      </c>
+      <c r="H175" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>260</v>
       </c>
@@ -4718,8 +6025,14 @@
       <c r="F176" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G176" t="s">
+        <v>341</v>
+      </c>
+      <c r="H176" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>260</v>
       </c>
@@ -4737,6 +6050,12 @@
       </c>
       <c r="F177" t="s">
         <v>261</v>
+      </c>
+      <c r="G177" t="s">
+        <v>341</v>
+      </c>
+      <c r="H177" s="2" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>